<commit_message>
Correction on the self assessment file
</commit_message>
<xml_diff>
--- a/artifacts/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint2.xlsx
+++ b/artifacts/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcaro\PI3\lapr3-2023-2024-group322_main\artifacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogoespiritosanto/ESINF/master/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE670B-BCB6-4A6C-95E1-28F1B284A812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277EABAE-9A76-D045-A392-5C47EDFB28BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1748,33 +1748,33 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.83203125" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1785,13 +1785,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
@@ -1813,7 +1813,7 @@
       <c r="S8" s="66"/>
       <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -1880,7 +1880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="63"/>
       <c r="C11" s="8">
         <v>1212044</v>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="63"/>
       <c r="C12" s="8">
         <v>1212047</v>
@@ -1973,7 +1973,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="63"/>
       <c r="C13" s="8">
         <v>1221720</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="63"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="63"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="63"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="63"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="63"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2113,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="63"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="63"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="63"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="63"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="63"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="64"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
@@ -2318,27 +2318,27 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2415,21 +2415,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="62" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="63"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
@@ -2485,7 +2485,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
@@ -2509,7 +2509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>3</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>4</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>5</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>6</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>7</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>9</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>9</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -2765,7 +2765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -2789,7 +2789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -2813,7 +2813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -2837,7 +2837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -2861,7 +2861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -2885,7 +2885,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -2909,7 +2909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -2933,7 +2933,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -2957,7 +2957,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -2981,7 +2981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -3005,7 +3005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -3074,24 +3074,24 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>37</v>
       </c>
@@ -3110,8 +3110,8 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>54</v>
       </c>
@@ -3365,7 +3365,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>60</v>
       </c>
@@ -3416,7 +3416,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -3494,7 +3494,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>66</v>
       </c>
@@ -3569,7 +3569,7 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -3588,26 +3588,26 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.6640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
@@ -3626,7 +3626,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>68</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>75</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>82</v>
       </c>
@@ -3880,7 +3880,7 @@
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>89</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>95</v>
       </c>
@@ -3982,7 +3982,7 @@
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>101</v>
       </c>
@@ -3990,11 +3990,11 @@
         <v>0.05</v>
       </c>
       <c r="C9" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -4010,7 +4010,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="55">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" s="59" t="s">
         <v>102</v>
@@ -4029,7 +4029,7 @@
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>106</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>112</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>118</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>119</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>126</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>4.1499999999999995</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>3.95</v>
+        <v>3.9</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
@@ -4362,14 +4362,14 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>16.599999999999998</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>15.8</v>
+        <v>15.600000000000001</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
@@ -4437,7 +4437,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -4452,12 +4452,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4645,15 +4642,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4678,17 +4686,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>